<commit_message>
adjustment to handguards and stocks
</commit_message>
<xml_diff>
--- a/changes/ak-handguards.xlsx
+++ b/changes/ak-handguards.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yifan\Documents\deadline-balancing\changes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A9465BA-004A-4578-94D1-7ED60821210B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73892A47-65C8-489C-8795-26C59986C34C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="147">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="150">
   <si>
     <t>new</t>
   </si>
@@ -474,6 +474,15 @@
   </si>
   <si>
     <t>Zenitco B-10L "Sport" + B-19</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>e</t>
   </si>
 </sst>
 </file>
@@ -957,8 +966,9 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1314,10 +1324,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R95"/>
+  <dimension ref="A1:T95"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" topLeftCell="A67" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="T74" sqref="T74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1758,17 +1768,17 @@
         <v>0.09</v>
       </c>
       <c r="E16">
+        <v>-6</v>
+      </c>
+      <c r="F16">
         <v>-5</v>
-      </c>
-      <c r="F16">
-        <v>-6</v>
       </c>
       <c r="M16">
         <v>1000</v>
       </c>
       <c r="N16">
         <f t="shared" si="0"/>
-        <v>17.799999999999997</v>
+        <v>18</v>
       </c>
       <c r="P16">
         <v>3.52</v>
@@ -1792,17 +1802,17 @@
         <v>0.09</v>
       </c>
       <c r="E17">
+        <v>-6</v>
+      </c>
+      <c r="F17">
         <v>-5</v>
-      </c>
-      <c r="F17">
-        <v>-6</v>
       </c>
       <c r="M17">
         <v>1000</v>
       </c>
       <c r="N17">
         <f t="shared" si="0"/>
-        <v>17.799999999999997</v>
+        <v>18</v>
       </c>
       <c r="Q17">
         <f t="shared" si="1"/>
@@ -2025,13 +2035,13 @@
         <v>56</v>
       </c>
       <c r="C25">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D25">
         <v>0.14000000000000001</v>
       </c>
       <c r="E25">
-        <v>-6</v>
+        <v>-7</v>
       </c>
       <c r="F25">
         <v>-7</v>
@@ -2041,7 +2051,7 @@
       </c>
       <c r="N25">
         <f t="shared" si="0"/>
-        <v>17.2</v>
+        <v>17</v>
       </c>
       <c r="P25">
         <v>16</v>
@@ -2062,13 +2072,13 @@
         <v>56</v>
       </c>
       <c r="C26">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D26">
         <v>0.14000000000000001</v>
       </c>
       <c r="E26">
-        <v>-6</v>
+        <v>-7</v>
       </c>
       <c r="F26">
         <v>-7</v>
@@ -2078,7 +2088,7 @@
       </c>
       <c r="N26">
         <f t="shared" si="0"/>
-        <v>17.2</v>
+        <v>17</v>
       </c>
       <c r="Q26">
         <f t="shared" si="1"/>
@@ -2093,23 +2103,23 @@
         <v>22</v>
       </c>
       <c r="C27">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D27">
         <v>0.17</v>
       </c>
       <c r="E27">
+        <v>-7</v>
+      </c>
+      <c r="F27">
         <v>-9</v>
-      </c>
-      <c r="F27">
-        <v>-8</v>
       </c>
       <c r="M27">
         <v>1200</v>
       </c>
       <c r="N27">
         <f>C27-D27*20-E27*0.8-F27*0.6-H27*5+I27*10+J27/300</f>
-        <v>17.600000000000001</v>
+        <v>17.599999999999998</v>
       </c>
       <c r="Q27">
         <f>P27*0.024</f>
@@ -2130,17 +2140,17 @@
         <v>0.24</v>
       </c>
       <c r="E28">
-        <v>-11</v>
+        <v>-10</v>
       </c>
       <c r="F28">
-        <v>-10</v>
+        <v>-12</v>
       </c>
       <c r="M28">
         <v>1600</v>
       </c>
       <c r="N28">
         <f t="shared" si="0"/>
-        <v>17</v>
+        <v>17.399999999999999</v>
       </c>
       <c r="P28">
         <v>10</v>
@@ -2158,13 +2168,13 @@
         <v>50</v>
       </c>
       <c r="C29">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D29">
         <v>0.15</v>
       </c>
       <c r="E29">
-        <v>-7</v>
+        <v>-8</v>
       </c>
       <c r="F29">
         <v>-4</v>
@@ -2174,7 +2184,7 @@
       </c>
       <c r="N29">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>17.8</v>
       </c>
       <c r="P29">
         <v>7.9</v>
@@ -2195,23 +2205,23 @@
         <v>52</v>
       </c>
       <c r="C30">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D30">
         <v>0.21</v>
       </c>
       <c r="E30">
-        <v>-9</v>
+        <v>-11</v>
       </c>
       <c r="F30">
-        <v>-6</v>
+        <v>-7</v>
       </c>
       <c r="M30">
         <v>1600</v>
       </c>
       <c r="N30">
         <f t="shared" si="0"/>
-        <v>17.600000000000001</v>
+        <v>17.8</v>
       </c>
       <c r="P30">
         <v>11.4</v>
@@ -2232,7 +2242,7 @@
         <v>46</v>
       </c>
       <c r="C31">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D31">
         <v>0.15</v>
@@ -2241,14 +2251,14 @@
         <v>-6</v>
       </c>
       <c r="F31">
-        <v>-6</v>
+        <v>-5</v>
       </c>
       <c r="M31">
         <v>1000</v>
       </c>
       <c r="N31">
         <f t="shared" si="0"/>
-        <v>17.399999999999999</v>
+        <v>17.8</v>
       </c>
       <c r="P31">
         <v>6.3493199999999996</v>
@@ -2266,7 +2276,7 @@
         <v>46</v>
       </c>
       <c r="C32">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D32">
         <v>0.15</v>
@@ -2275,14 +2285,14 @@
         <v>-6</v>
       </c>
       <c r="F32">
-        <v>-6</v>
+        <v>-5</v>
       </c>
       <c r="M32">
         <v>1000</v>
       </c>
       <c r="N32">
         <f t="shared" si="0"/>
-        <v>17.399999999999999</v>
+        <v>17.8</v>
       </c>
       <c r="Q32">
         <f t="shared" si="1"/>
@@ -2297,23 +2307,23 @@
         <v>34</v>
       </c>
       <c r="C33">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D33">
         <v>0.23</v>
       </c>
       <c r="E33">
-        <v>-9</v>
+        <v>-10</v>
       </c>
       <c r="F33">
-        <v>-10</v>
+        <v>-11</v>
       </c>
       <c r="M33">
         <v>1500</v>
       </c>
       <c r="N33">
         <f>C33-D33*20-E33*0.8-F33*0.6-H33*5+I33*10+J33/300</f>
-        <v>17.600000000000001</v>
+        <v>18</v>
       </c>
       <c r="P33">
         <v>9.5239799999999999</v>
@@ -2331,7 +2341,7 @@
         <v>48</v>
       </c>
       <c r="C34">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D34">
         <v>0.09</v>
@@ -2340,14 +2350,14 @@
         <v>-7</v>
       </c>
       <c r="F34">
-        <v>-7</v>
+        <v>-6</v>
       </c>
       <c r="M34">
         <v>1100</v>
       </c>
       <c r="N34">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>18.399999999999999</v>
       </c>
       <c r="P34">
         <v>3.1746599999999998</v>
@@ -2365,7 +2375,7 @@
         <v>48</v>
       </c>
       <c r="C35">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D35">
         <v>0.09</v>
@@ -2374,14 +2384,14 @@
         <v>-7</v>
       </c>
       <c r="F35">
-        <v>-7</v>
+        <v>-6</v>
       </c>
       <c r="M35">
         <v>1100</v>
       </c>
       <c r="N35">
         <f t="shared" si="0"/>
-        <v>18</v>
+        <v>18.399999999999999</v>
       </c>
       <c r="Q35">
         <f t="shared" si="1"/>
@@ -2467,7 +2477,7 @@
         <v>8</v>
       </c>
       <c r="D38">
-        <v>0.1</v>
+        <v>0.11</v>
       </c>
       <c r="E38">
         <v>-5</v>
@@ -2480,7 +2490,7 @@
       </c>
       <c r="N38">
         <f t="shared" si="0"/>
-        <v>16.600000000000001</v>
+        <v>16.399999999999999</v>
       </c>
       <c r="Q38">
         <f t="shared" si="1"/>
@@ -2658,23 +2668,23 @@
         <v>130</v>
       </c>
       <c r="C46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D46">
         <v>0.04</v>
       </c>
       <c r="E46">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="F46">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
       <c r="M46">
         <v>0</v>
       </c>
       <c r="N46">
         <f>C46-D46*20-E46*0.8-F46*0.6-H46*5+I46*10+J46/300</f>
-        <v>0.49999999999999994</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="47" spans="1:17" x14ac:dyDescent="0.25">
@@ -2716,7 +2726,7 @@
         <v>42</v>
       </c>
       <c r="C48">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D48">
         <v>0.04</v>
@@ -2725,14 +2735,14 @@
         <v>-0.5</v>
       </c>
       <c r="F48">
-        <v>-1</v>
+        <v>0</v>
       </c>
       <c r="M48">
         <v>500</v>
       </c>
       <c r="N48">
         <f t="shared" si="0"/>
-        <v>0.7</v>
+        <v>0.6</v>
       </c>
       <c r="P48">
         <v>1.2725919999999999</v>
@@ -2750,23 +2760,23 @@
         <v>82</v>
       </c>
       <c r="C49">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
       <c r="D49">
         <v>0.03</v>
       </c>
       <c r="E49">
+        <v>-2</v>
+      </c>
+      <c r="F49">
         <v>-1</v>
-      </c>
-      <c r="F49">
-        <v>-1.5</v>
       </c>
       <c r="M49">
         <v>400</v>
       </c>
       <c r="N49">
         <f t="shared" si="0"/>
-        <v>0.59999999999999987</v>
+        <v>0.6</v>
       </c>
       <c r="Q49">
         <f t="shared" si="1"/>
@@ -2979,24 +2989,24 @@
       <c r="B57" t="s">
         <v>112</v>
       </c>
-      <c r="C57">
-        <v>1</v>
+      <c r="C57" s="1">
+        <v>0</v>
       </c>
       <c r="D57">
         <v>0.08</v>
       </c>
       <c r="E57">
-        <v>-1</v>
+        <v>-1.5</v>
       </c>
       <c r="F57">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="M57">
         <v>750</v>
       </c>
       <c r="N57">
         <f t="shared" si="0"/>
-        <v>0.79999999999999993</v>
+        <v>0.8</v>
       </c>
       <c r="P57">
         <v>3.1746599999999998</v>
@@ -3014,16 +3024,16 @@
         <v>110</v>
       </c>
       <c r="C58">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D58">
         <v>0.06</v>
       </c>
       <c r="E58">
-        <v>-0.5</v>
+        <v>-1</v>
       </c>
       <c r="F58">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="M58">
         <v>800</v>
@@ -3116,7 +3126,7 @@
         <v>95</v>
       </c>
       <c r="C61">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D61">
         <v>0.14000000000000001</v>
@@ -3125,14 +3135,14 @@
         <v>-2</v>
       </c>
       <c r="F61">
-        <v>-4</v>
+        <v>-3</v>
       </c>
       <c r="M61">
         <v>1200</v>
       </c>
       <c r="N61">
         <f t="shared" si="0"/>
-        <v>1.1999999999999997</v>
+        <v>1.5999999999999996</v>
       </c>
       <c r="P61">
         <v>4.6561680000000001</v>
@@ -3150,7 +3160,7 @@
         <v>124</v>
       </c>
       <c r="C62">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D62">
         <v>0.13</v>
@@ -3159,14 +3169,14 @@
         <v>-3</v>
       </c>
       <c r="F62">
-        <v>-2</v>
+        <v>-1</v>
       </c>
       <c r="M62">
         <v>1600</v>
       </c>
       <c r="N62">
         <f t="shared" si="0"/>
-        <v>1.0000000000000002</v>
+        <v>1.4000000000000004</v>
       </c>
       <c r="P62">
         <v>5.5732920000000004</v>
@@ -3184,7 +3194,7 @@
         <v>108</v>
       </c>
       <c r="C63">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D63">
         <v>0.05</v>
@@ -3193,14 +3203,14 @@
         <v>0</v>
       </c>
       <c r="F63">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="M63">
         <v>600</v>
       </c>
       <c r="N63">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>-0.4</v>
       </c>
       <c r="P63">
         <v>2.1517140000000001</v>
@@ -3218,7 +3228,7 @@
         <v>122</v>
       </c>
       <c r="C64">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D64">
         <v>7.0000000000000007E-2</v>
@@ -3227,14 +3237,14 @@
         <v>-1</v>
       </c>
       <c r="F64">
-        <v>0</v>
+        <v>-1</v>
       </c>
       <c r="M64">
         <v>600</v>
       </c>
       <c r="N64">
         <f t="shared" si="0"/>
-        <v>0.39999999999999991</v>
+        <v>-1.1102230246251565E-16</v>
       </c>
       <c r="P64">
         <v>2.2928099999999998</v>
@@ -3244,7 +3254,7 @@
         <v>5.5027439999999997E-2</v>
       </c>
     </row>
-    <row r="65" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>125</v>
       </c>
@@ -3278,7 +3288,7 @@
         <v>4.4021952000000003E-2</v>
       </c>
     </row>
-    <row r="66" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>100</v>
       </c>
@@ -3309,7 +3319,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>102</v>
       </c>
@@ -3317,30 +3327,30 @@
         <v>103</v>
       </c>
       <c r="C67">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D67">
-        <v>0.12</v>
+        <v>0.13</v>
       </c>
       <c r="E67">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="F67">
-        <v>-1</v>
+        <v>-2</v>
       </c>
       <c r="M67">
         <v>0</v>
       </c>
       <c r="N67">
         <f t="shared" si="0"/>
-        <v>1.1102230246251565E-16</v>
+        <v>0.19999999999999996</v>
       </c>
       <c r="Q67">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
     </row>
-    <row r="68" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B68" t="s">
         <v>133</v>
       </c>
@@ -3349,7 +3359,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>119</v>
       </c>
@@ -3370,7 +3380,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="70" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>127</v>
       </c>
@@ -3397,13 +3407,13 @@
         <v>6.1999999999999993</v>
       </c>
     </row>
-    <row r="71" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:20" x14ac:dyDescent="0.25">
       <c r="N71">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
     </row>
-    <row r="72" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
         <v>134</v>
       </c>
@@ -3450,7 +3460,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="73" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
         <v>28</v>
       </c>
@@ -3514,8 +3524,11 @@
         <f t="shared" si="3"/>
         <v>0.12</v>
       </c>
-    </row>
-    <row r="74" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="T73" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="74" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B74" t="s">
         <v>36</v>
       </c>
@@ -3579,14 +3592,17 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="75" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="T74" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="75" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B75" t="s">
         <v>114</v>
       </c>
       <c r="C75">
         <f t="shared" ref="C75:Q75" si="5">C10+C46</f>
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D75">
         <f t="shared" si="5"/>
@@ -3594,11 +3610,11 @@
       </c>
       <c r="E75">
         <f t="shared" si="5"/>
-        <v>-6</v>
+        <v>-7</v>
       </c>
       <c r="F75">
         <f t="shared" si="5"/>
-        <v>-8.5</v>
+        <v>-9</v>
       </c>
       <c r="G75">
         <f t="shared" si="5"/>
@@ -3630,7 +3646,7 @@
       </c>
       <c r="N75">
         <f t="shared" si="5"/>
-        <v>24.1</v>
+        <v>24.200000000000003</v>
       </c>
       <c r="O75">
         <f t="shared" si="5"/>
@@ -3644,8 +3660,11 @@
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="76" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="T75" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="76" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B76" t="s">
         <v>54</v>
       </c>
@@ -3709,8 +3728,11 @@
         <f t="shared" si="6"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="77" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="T76" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="77" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B77" t="s">
         <v>139</v>
       </c>
@@ -3774,14 +3796,17 @@
         <f t="shared" si="7"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="78" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="T77" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="78" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B78" t="s">
         <v>18</v>
       </c>
       <c r="C78">
         <f t="shared" ref="C78:Q78" si="8">C16+C49</f>
-        <v>11.5</v>
+        <v>11</v>
       </c>
       <c r="D78">
         <f t="shared" si="8"/>
@@ -3789,11 +3814,11 @@
       </c>
       <c r="E78">
         <f t="shared" si="8"/>
-        <v>-6</v>
+        <v>-8</v>
       </c>
       <c r="F78">
         <f t="shared" si="8"/>
-        <v>-7.5</v>
+        <v>-6</v>
       </c>
       <c r="G78">
         <f t="shared" si="8"/>
@@ -3825,7 +3850,7 @@
       </c>
       <c r="N78">
         <f t="shared" si="8"/>
-        <v>18.399999999999999</v>
+        <v>18.600000000000001</v>
       </c>
       <c r="O78">
         <f t="shared" si="8"/>
@@ -3839,14 +3864,17 @@
         <f t="shared" si="8"/>
         <v>8.448E-2</v>
       </c>
-    </row>
-    <row r="79" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="T78" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="79" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B79" t="s">
         <v>42</v>
       </c>
       <c r="C79">
         <f t="shared" ref="C79:Q79" si="9">C18+C48</f>
-        <v>15.5</v>
+        <v>16</v>
       </c>
       <c r="D79">
         <f t="shared" si="9"/>
@@ -3858,7 +3886,7 @@
       </c>
       <c r="F79">
         <f t="shared" si="9"/>
-        <v>-5</v>
+        <v>-4</v>
       </c>
       <c r="G79">
         <f t="shared" si="9"/>
@@ -3890,7 +3918,7 @@
       </c>
       <c r="N79">
         <f t="shared" si="9"/>
-        <v>17.7</v>
+        <v>17.600000000000001</v>
       </c>
       <c r="O79">
         <f t="shared" si="9"/>
@@ -3904,14 +3932,17 @@
         <f t="shared" si="9"/>
         <v>0.21774220799999999</v>
       </c>
-    </row>
-    <row r="80" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="T79" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="80" spans="1:20" x14ac:dyDescent="0.25">
       <c r="B80" t="s">
         <v>24</v>
       </c>
       <c r="C80">
         <f t="shared" ref="C80:Q80" si="10">C20+C48</f>
-        <v>16.5</v>
+        <v>17</v>
       </c>
       <c r="D80">
         <f t="shared" si="10"/>
@@ -3923,7 +3954,7 @@
       </c>
       <c r="F80">
         <f t="shared" si="10"/>
-        <v>-7</v>
+        <v>-6</v>
       </c>
       <c r="G80">
         <f t="shared" si="10"/>
@@ -3955,7 +3986,7 @@
       </c>
       <c r="N80">
         <f t="shared" si="10"/>
-        <v>17.499999999999996</v>
+        <v>17.399999999999999</v>
       </c>
       <c r="O80">
         <f t="shared" si="10"/>
@@ -3969,8 +4000,11 @@
         <f t="shared" si="10"/>
         <v>0.3624</v>
       </c>
-    </row>
-    <row r="81" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="T80" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="81" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B81" t="s">
         <v>39</v>
       </c>
@@ -4034,14 +4068,17 @@
         <f t="shared" si="11"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="82" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="T81" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="82" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B82" t="s">
         <v>138</v>
       </c>
       <c r="C82">
         <f t="shared" ref="C82:Q82" si="12">C25+C51+C69</f>
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D82">
         <f t="shared" si="12"/>
@@ -4049,7 +4086,7 @@
       </c>
       <c r="E82">
         <f t="shared" si="12"/>
-        <v>-8</v>
+        <v>-9</v>
       </c>
       <c r="F82">
         <f t="shared" si="12"/>
@@ -4085,7 +4122,7 @@
       </c>
       <c r="N82">
         <f t="shared" si="12"/>
-        <v>18</v>
+        <v>17.8</v>
       </c>
       <c r="O82">
         <f t="shared" si="12"/>
@@ -4099,14 +4136,17 @@
         <f t="shared" si="12"/>
         <v>0.38400000000000001</v>
       </c>
-    </row>
-    <row r="83" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="T82" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="83" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B83" t="s">
         <v>22</v>
       </c>
       <c r="C83">
         <f t="shared" ref="C83:Q83" si="13">C27+C52</f>
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D83">
         <f t="shared" si="13"/>
@@ -4114,11 +4154,11 @@
       </c>
       <c r="E83">
         <f t="shared" si="13"/>
-        <v>-10</v>
+        <v>-8</v>
       </c>
       <c r="F83">
         <f t="shared" si="13"/>
-        <v>-10</v>
+        <v>-11</v>
       </c>
       <c r="G83">
         <f t="shared" si="13"/>
@@ -4150,7 +4190,7 @@
       </c>
       <c r="N83">
         <f t="shared" si="13"/>
-        <v>18.400000000000002</v>
+        <v>18.399999999999999</v>
       </c>
       <c r="O83">
         <f t="shared" si="13"/>
@@ -4164,8 +4204,11 @@
         <f t="shared" si="13"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="84" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="T83" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="84" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B84" t="s">
         <v>20</v>
       </c>
@@ -4179,11 +4222,11 @@
       </c>
       <c r="E84">
         <f t="shared" si="14"/>
-        <v>-12</v>
+        <v>-11</v>
       </c>
       <c r="F84">
         <f t="shared" si="14"/>
-        <v>-12</v>
+        <v>-14</v>
       </c>
       <c r="G84">
         <f t="shared" si="14"/>
@@ -4215,7 +4258,7 @@
       </c>
       <c r="N84">
         <f t="shared" si="14"/>
-        <v>17.8</v>
+        <v>18.2</v>
       </c>
       <c r="O84">
         <f t="shared" si="14"/>
@@ -4229,14 +4272,17 @@
         <f t="shared" si="14"/>
         <v>0.24</v>
       </c>
-    </row>
-    <row r="85" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="T84" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="85" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B85" t="s">
         <v>137</v>
       </c>
       <c r="C85">
         <f t="shared" ref="C85:Q85" si="15">C29+C55</f>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D85">
         <f t="shared" si="15"/>
@@ -4244,7 +4290,7 @@
       </c>
       <c r="E85">
         <f t="shared" si="15"/>
-        <v>-9</v>
+        <v>-10</v>
       </c>
       <c r="F85">
         <f t="shared" si="15"/>
@@ -4280,7 +4326,7 @@
       </c>
       <c r="N85">
         <f t="shared" si="15"/>
-        <v>18.8</v>
+        <v>18.600000000000001</v>
       </c>
       <c r="O85">
         <f t="shared" si="15"/>
@@ -4294,14 +4340,17 @@
         <f t="shared" si="15"/>
         <v>0.18960000000000002</v>
       </c>
-    </row>
-    <row r="86" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="T85" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="86" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B86" t="s">
         <v>136</v>
       </c>
       <c r="C86">
         <f t="shared" ref="C86:Q86" si="16">C30+C56</f>
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="D86">
         <f t="shared" si="16"/>
@@ -4309,11 +4358,11 @@
       </c>
       <c r="E86">
         <f t="shared" si="16"/>
-        <v>-11</v>
+        <v>-13</v>
       </c>
       <c r="F86">
         <f t="shared" si="16"/>
-        <v>-7</v>
+        <v>-8</v>
       </c>
       <c r="G86">
         <f t="shared" si="16"/>
@@ -4345,7 +4394,7 @@
       </c>
       <c r="N86">
         <f t="shared" si="16"/>
-        <v>18.400000000000002</v>
+        <v>18.600000000000001</v>
       </c>
       <c r="O86">
         <f t="shared" si="16"/>
@@ -4359,8 +4408,11 @@
         <f t="shared" si="16"/>
         <v>0.27360000000000001</v>
       </c>
-    </row>
-    <row r="87" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="T86" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="87" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B87" t="s">
         <v>144</v>
       </c>
@@ -4374,7 +4426,7 @@
       </c>
       <c r="E87">
         <f t="shared" si="17"/>
-        <v>-7</v>
+        <v>-7.5</v>
       </c>
       <c r="F87">
         <f t="shared" si="17"/>
@@ -4410,7 +4462,7 @@
       </c>
       <c r="N87">
         <f t="shared" si="17"/>
-        <v>18.2</v>
+        <v>18.600000000000001</v>
       </c>
       <c r="O87">
         <f t="shared" si="17"/>
@@ -4424,14 +4476,17 @@
         <f t="shared" si="17"/>
         <v>0.22857551999999998</v>
       </c>
-    </row>
-    <row r="88" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="T87" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="88" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
         <v>145</v>
       </c>
       <c r="C88">
         <f t="shared" ref="C88:Q88" si="18">C33+C59</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D88">
         <f t="shared" si="18"/>
@@ -4439,11 +4494,11 @@
       </c>
       <c r="E88">
         <f t="shared" si="18"/>
-        <v>-11</v>
+        <v>-12</v>
       </c>
       <c r="F88">
         <f t="shared" si="18"/>
-        <v>-12</v>
+        <v>-13</v>
       </c>
       <c r="G88">
         <f t="shared" si="18"/>
@@ -4475,7 +4530,7 @@
       </c>
       <c r="N88">
         <f t="shared" si="18"/>
-        <v>18.400000000000002</v>
+        <v>18.8</v>
       </c>
       <c r="O88">
         <f t="shared" si="18"/>
@@ -4489,8 +4544,11 @@
         <f t="shared" si="18"/>
         <v>0.326778336</v>
       </c>
-    </row>
-    <row r="89" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="T88" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="89" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B89" t="s">
         <v>146</v>
       </c>
@@ -4504,7 +4562,7 @@
       </c>
       <c r="E89">
         <f t="shared" si="19"/>
-        <v>-8</v>
+        <v>-8.5</v>
       </c>
       <c r="F89">
         <f t="shared" si="19"/>
@@ -4540,7 +4598,7 @@
       </c>
       <c r="N89">
         <f t="shared" si="19"/>
-        <v>18.8</v>
+        <v>19.2</v>
       </c>
       <c r="O89">
         <f t="shared" si="19"/>
@@ -4554,14 +4612,17 @@
         <f t="shared" si="19"/>
         <v>0.15238367999999999</v>
       </c>
-    </row>
-    <row r="90" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="T89" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="90" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B90" t="s">
         <v>140</v>
       </c>
       <c r="C90">
         <f>C34+C61+C63</f>
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D90">
         <f t="shared" ref="D90:Q90" si="20">D34+D61+D63</f>
@@ -4573,7 +4634,7 @@
       </c>
       <c r="F90">
         <f t="shared" si="20"/>
-        <v>-11</v>
+        <v>-10</v>
       </c>
       <c r="G90">
         <f t="shared" si="20"/>
@@ -4605,7 +4666,7 @@
       </c>
       <c r="N90">
         <f t="shared" si="20"/>
-        <v>19.2</v>
+        <v>19.600000000000001</v>
       </c>
       <c r="O90">
         <f t="shared" si="20"/>
@@ -4622,14 +4683,17 @@
       <c r="R90">
         <v>0.284449536</v>
       </c>
-    </row>
-    <row r="91" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="T90" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="91" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B91" t="s">
         <v>141</v>
       </c>
       <c r="C91">
         <f>C34+C62+C64+C65</f>
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D91">
         <f t="shared" ref="D91:Q91" si="21">D34+D62+D64+D65</f>
@@ -4641,7 +4705,7 @@
       </c>
       <c r="F91">
         <f t="shared" si="21"/>
-        <v>-9</v>
+        <v>-8</v>
       </c>
       <c r="G91">
         <f t="shared" si="21"/>
@@ -4673,7 +4737,7 @@
       </c>
       <c r="N91">
         <f t="shared" si="21"/>
-        <v>19.599999999999998</v>
+        <v>19.999999999999996</v>
       </c>
       <c r="O91">
         <f t="shared" si="21"/>
@@ -4690,14 +4754,17 @@
       <c r="R91">
         <v>0.32593176000000001</v>
       </c>
-    </row>
-    <row r="92" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="T91" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="92" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B92" t="s">
         <v>142</v>
       </c>
       <c r="C92">
         <f>C36+C57</f>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D92">
         <f t="shared" ref="D92:Q92" si="22">D36+D57</f>
@@ -4705,11 +4772,11 @@
       </c>
       <c r="E92">
         <f t="shared" si="22"/>
-        <v>-6</v>
+        <v>-6.5</v>
       </c>
       <c r="F92">
         <f t="shared" si="22"/>
-        <v>-7</v>
+        <v>-8</v>
       </c>
       <c r="G92">
         <f t="shared" si="22"/>
@@ -4755,14 +4822,17 @@
         <f t="shared" si="22"/>
         <v>0.19894535999999999</v>
       </c>
-    </row>
-    <row r="93" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="T92" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="93" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B93" t="s">
         <v>143</v>
       </c>
       <c r="C93">
         <f>C37+C57</f>
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D93">
         <f t="shared" ref="D93:Q93" si="23">D37+D57</f>
@@ -4770,11 +4840,11 @@
       </c>
       <c r="E93">
         <f t="shared" si="23"/>
-        <v>-6</v>
+        <v>-6.5</v>
       </c>
       <c r="F93">
         <f t="shared" si="23"/>
-        <v>-6</v>
+        <v>-7</v>
       </c>
       <c r="G93">
         <f t="shared" si="23"/>
@@ -4820,26 +4890,29 @@
         <f t="shared" si="23"/>
         <v>0.15661656000000002</v>
       </c>
-    </row>
-    <row r="94" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="T93" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="94" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B94" t="s">
         <v>26</v>
       </c>
       <c r="C94">
         <f t="shared" ref="C94:Q94" si="24">C38+C66+C67</f>
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D94">
         <f t="shared" si="24"/>
-        <v>0.29000000000000004</v>
+        <v>0.31</v>
       </c>
       <c r="E94">
         <f t="shared" si="24"/>
-        <v>-7</v>
+        <v>-8</v>
       </c>
       <c r="F94">
         <f t="shared" si="24"/>
-        <v>-14</v>
+        <v>-15</v>
       </c>
       <c r="G94">
         <f t="shared" si="24"/>
@@ -4871,7 +4944,7 @@
       </c>
       <c r="N94">
         <f t="shared" si="24"/>
-        <v>17.200000000000003</v>
+        <v>17.2</v>
       </c>
       <c r="O94">
         <f t="shared" si="24"/>
@@ -4885,8 +4958,11 @@
         <f t="shared" si="24"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="95" spans="2:18" x14ac:dyDescent="0.25">
+      <c r="T94" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="95" spans="2:20" x14ac:dyDescent="0.25">
       <c r="B95" t="str">
         <f>B40</f>
         <v>TDI Arms X47 Rail System</v>
@@ -4950,6 +5026,9 @@
       <c r="Q95">
         <f t="shared" si="25"/>
         <v>0.35544000000000003</v>
+      </c>
+      <c r="T95" t="s">
+        <v>147</v>
       </c>
     </row>
   </sheetData>

</xml_diff>